<commit_message>
actualizacion de transacciones y pedidos 19/9/2024
</commit_message>
<xml_diff>
--- a/uploads/excel/newOrder.xlsx
+++ b/uploads/excel/newOrder.xlsx
@@ -1815,32 +1815,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100DFDABE89AEBAFC40B2417B437CFB6AC3" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b0cd73b5ccf93356e9cd4fc48e1f9794">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="74d56a54-6253-49af-9dde-609db7d41aef" xmlns:ns4="15c23791-412b-494d-9514-6bfd1dc7436b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dcc312e3b1a27c29ed239405870c257a" ns3:_="" ns4:_="">
-    <xsd:import namespace="74d56a54-6253-49af-9dde-609db7d41aef"/>
-    <xsd:import namespace="15c23791-412b-494d-9514-6bfd1dc7436b"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008C7E4CFE7976B14B81D4C5D1DD1E52C5" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="607fa83e4d6b3a1bf15103989bdc0471">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78368757-d54f-4d5f-9d37-16d0676caa23" xmlns:ns3="a56850d5-d898-4bfd-9b80-991e91e89fb2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17c92c7783743ce619547fd81eb29b0c" ns2:_="" ns3:_="">
+    <xsd:import namespace="78368757-d54f-4d5f-9d37-16d0676caa23"/>
+    <xsd:import namespace="a56850d5-d898-4bfd-9b80-991e91e89fb2"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:_activity" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1848,7 +1843,7 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="74d56a54-6253-49af-9dde-609db7d41aef" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="78368757-d54f-4d5f-9d37-16d0676caa23" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
@@ -1861,97 +1856,64 @@
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="be3ca0f0-b902-41e1-af55-471844d5da19" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_activity" ma:index="16" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="20" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSystemTags" ma:index="21" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="23" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="15c23791-412b-494d-9514-6bfd1dc7436b" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a56850d5-d898-4bfd-9b80-991e91e89fb2" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="17" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{6b7a86e6-2089-443a-9e57-7d6663bab24e}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="a56850d5-d898-4bfd-9b80-991e91e89fb2">
       <xsd:complexType>
         <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
+          <xsd:extension base="dms:MultiChoiceLookup">
             <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
             </xsd:sequence>
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="18" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="19" nillable="true" ma:displayName="Hash de la sugerencia para compartir" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -2065,28 +2027,16 @@
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
-    <_activity xmlns="74d56a54-6253-49af-9dde-609db7d41aef" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="78368757-d54f-4d5f-9d37-16d0676caa23">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a56850d5-d898-4bfd-9b80-991e91e89fb2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AFBE616-7E4D-463F-9414-8B823D297FF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="74d56a54-6253-49af-9dde-609db7d41aef"/>
-    <ds:schemaRef ds:uri="15c23791-412b-494d-9514-6bfd1dc7436b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37FB4BA3-B18F-4632-82A9-BEC105D0AACE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>